<commit_message>
batch corrected by rna extraction date and sorting date. Looks like that had a fairly substantial batch effect. non-infected and infected animals now correctly cluster together. cd8_depleted and non-depleted non-infected animals cluster separately. Data quality looks good
</commit_message>
<xml_diff>
--- a/data/library_info.xlsx
+++ b/data/library_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewding/Desktop/Projects/2023 BrdU RNAseq/Analyses/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88FAFE5B-672B-A84D-BE93-8DA24A0F7077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0233EF-1614-974B-BB64-D4E37652A8F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16160" yWindow="0" windowWidth="13040" windowHeight="15140" xr2:uid="{80E030B8-BC9B-3D4F-89F4-4C59C10CB779}"/>
+    <workbookView xWindow="1940" yWindow="0" windowWidth="27240" windowHeight="15140" xr2:uid="{80E030B8-BC9B-3D4F-89F4-4C59C10CB779}"/>
   </bookViews>
   <sheets>
     <sheet name="sample info" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Sample checklist'!$A$1:$J$25</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'sample info'!$A$1:$CU$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'sample info'!$A$1:$CU$41</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Sample checklist'!$A$1:$G$25</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -663,11 +663,12 @@
   <dimension ref="A1:CU41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="4" max="6" width="10.83203125" customWidth="1"/>
     <col min="11" max="11" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20.1640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -760,7 +761,7 @@
         <v>352</v>
       </c>
       <c r="M2">
-        <f>K2*((1*10^6)/(L2*660))</f>
+        <f t="shared" ref="M2:M41" si="0">K2*((1*10^6)/(L2*660))</f>
         <v>134.29752066115702</v>
       </c>
       <c r="N2" s="1">
@@ -811,7 +812,7 @@
         <v>345</v>
       </c>
       <c r="M3">
-        <f>K3*((1*10^6)/(L3*660))</f>
+        <f t="shared" si="0"/>
         <v>167.76460254721127</v>
       </c>
       <c r="N3" s="1">
@@ -862,7 +863,7 @@
         <v>336</v>
       </c>
       <c r="M4">
-        <f>K4*((1*10^6)/(L4*660))</f>
+        <f t="shared" si="0"/>
         <v>122.65512265512265</v>
       </c>
       <c r="N4" s="1">
@@ -913,7 +914,7 @@
         <v>326</v>
       </c>
       <c r="M5">
-        <f>K5*((1*10^6)/(L5*660))</f>
+        <f t="shared" si="0"/>
         <v>142.21974344673734</v>
       </c>
       <c r="N5" s="1">
@@ -964,7 +965,7 @@
         <v>333</v>
       </c>
       <c r="M6">
-        <f>K6*((1*10^6)/(L6*660))</f>
+        <f t="shared" si="0"/>
         <v>149.24014924014921</v>
       </c>
       <c r="N6" s="1">
@@ -1015,7 +1016,7 @@
         <v>347</v>
       </c>
       <c r="M7">
-        <f>K7*((1*10^6)/(L7*660))</f>
+        <f t="shared" si="0"/>
         <v>114.40048904025851</v>
       </c>
       <c r="N7" s="1">
@@ -1066,7 +1067,7 @@
         <v>370</v>
       </c>
       <c r="M8">
-        <f>K8*((1*10^6)/(L8*660))</f>
+        <f t="shared" si="0"/>
         <v>109.74610974610974</v>
       </c>
       <c r="N8" s="1">
@@ -1117,7 +1118,7 @@
         <v>369</v>
       </c>
       <c r="M9">
-        <f>K9*((1*10^6)/(L9*660))</f>
+        <f t="shared" si="0"/>
         <v>95.26155867619282</v>
       </c>
       <c r="N9" s="1">
@@ -1168,7 +1169,7 @@
         <v>391</v>
       </c>
       <c r="M10">
-        <f>K10*((1*10^6)/(L10*660))</f>
+        <f t="shared" si="0"/>
         <v>82.151437650158869</v>
       </c>
       <c r="N10" s="1">
@@ -1219,7 +1220,7 @@
         <v>365</v>
       </c>
       <c r="M11">
-        <f>K11*((1*10^6)/(L11*660))</f>
+        <f t="shared" si="0"/>
         <v>67.247820672478198</v>
       </c>
       <c r="N11" s="1">
@@ -1270,7 +1271,7 @@
         <v>353</v>
       </c>
       <c r="M12">
-        <f>K12*((1*10^6)/(L12*660))</f>
+        <f t="shared" si="0"/>
         <v>102.15469138981888</v>
       </c>
       <c r="N12" s="1">
@@ -1321,7 +1322,7 @@
         <v>409</v>
       </c>
       <c r="M13">
-        <f>K13*((1*10^6)/(L13*660))</f>
+        <f t="shared" si="0"/>
         <v>68.533748240349709</v>
       </c>
       <c r="N13" s="1">
@@ -1372,7 +1373,7 @@
         <v>393</v>
       </c>
       <c r="M14">
-        <f>K14*((1*10^6)/(L14*660))</f>
+        <f t="shared" si="0"/>
         <v>53.589328398488711</v>
       </c>
       <c r="N14" s="1">
@@ -1423,7 +1424,7 @@
         <v>400</v>
       </c>
       <c r="M15">
-        <f>K15*((1*10^6)/(L15*660))</f>
+        <f t="shared" si="0"/>
         <v>48.863636363636367</v>
       </c>
       <c r="N15" s="1">
@@ -1474,7 +1475,7 @@
         <v>288</v>
       </c>
       <c r="M16">
-        <f>K16*((1*10^6)/(L16*660))</f>
+        <f t="shared" si="0"/>
         <v>97.32744107744108</v>
       </c>
       <c r="N16" s="1">
@@ -1525,7 +1526,7 @@
         <v>314</v>
       </c>
       <c r="M17">
-        <f>K17*((1*10^6)/(L17*660))</f>
+        <f t="shared" si="0"/>
         <v>260.56745801968731</v>
       </c>
       <c r="N17" s="1">
@@ -1577,7 +1578,7 @@
         <v>400</v>
       </c>
       <c r="M18">
-        <f>K18*((1*10^6)/(L18*660))</f>
+        <f t="shared" si="0"/>
         <v>89.77272727272728</v>
       </c>
       <c r="N18" s="1">
@@ -1628,7 +1629,7 @@
         <v>299</v>
       </c>
       <c r="M19">
-        <f>K19*((1*10^6)/(L19*660))</f>
+        <f t="shared" si="0"/>
         <v>198.64193777237256</v>
       </c>
       <c r="N19" s="1">
@@ -1680,7 +1681,7 @@
         <v>263</v>
       </c>
       <c r="M20">
-        <f>K20*((1*10^6)/(L20*660))</f>
+        <f t="shared" si="0"/>
         <v>158.42839036755387</v>
       </c>
       <c r="N20" s="1">
@@ -1731,7 +1732,7 @@
         <v>383</v>
       </c>
       <c r="M21">
-        <f>K21*((1*10^6)/(L21*660))</f>
+        <f t="shared" si="0"/>
         <v>118.28467442044465</v>
       </c>
       <c r="N21" s="1">
@@ -1783,7 +1784,7 @@
         <v>345</v>
       </c>
       <c r="M22">
-        <f>K22*((1*10^6)/(L22*660))</f>
+        <f t="shared" si="0"/>
         <v>162.93368467281513</v>
       </c>
       <c r="N22" s="1">
@@ -1834,7 +1835,7 @@
         <v>375</v>
       </c>
       <c r="M23">
-        <f>K23*((1*10^6)/(L23*660))</f>
+        <f t="shared" si="0"/>
         <v>205.25252525252526</v>
       </c>
       <c r="N23" s="1">
@@ -1885,7 +1886,7 @@
         <v>348</v>
       </c>
       <c r="M24">
-        <f>K24*((1*10^6)/(L24*660))</f>
+        <f t="shared" si="0"/>
         <v>36.224312086381047</v>
       </c>
       <c r="N24" s="1">
@@ -1936,7 +1937,7 @@
         <v>344</v>
       </c>
       <c r="M25">
-        <f>K25*((1*10^6)/(L25*660))</f>
+        <f t="shared" si="0"/>
         <v>56.377730796335449</v>
       </c>
       <c r="N25" s="1">
@@ -1987,7 +1988,7 @@
         <v>343</v>
       </c>
       <c r="M26">
-        <f>K26*((1*10^6)/(L26*660))</f>
+        <f t="shared" si="0"/>
         <v>57.867302765261954</v>
       </c>
       <c r="N26" s="1">
@@ -2038,7 +2039,7 @@
         <v>292</v>
       </c>
       <c r="M27">
-        <f>K27*((1*10^6)/(L27*660))</f>
+        <f t="shared" si="0"/>
         <v>26.359485263594852</v>
       </c>
       <c r="N27" s="1">
@@ -2089,7 +2090,7 @@
         <v>284</v>
       </c>
       <c r="M28">
-        <f>K28*((1*10^6)/(L28*660))</f>
+        <f t="shared" si="0"/>
         <v>29.449423815620996</v>
       </c>
       <c r="N28" s="1">
@@ -2140,7 +2141,7 @@
         <v>339</v>
       </c>
       <c r="M29">
-        <f>K29*((1*10^6)/(L29*660))</f>
+        <f t="shared" si="0"/>
         <v>71.958523285956929</v>
       </c>
       <c r="N29" s="1">
@@ -2173,10 +2174,10 @@
         <v>30</v>
       </c>
       <c r="G30" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H30" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I30">
         <v>3133</v>
@@ -2191,7 +2192,7 @@
         <v>388</v>
       </c>
       <c r="M30">
-        <f>K30*((1*10^6)/(L30*660))</f>
+        <f t="shared" si="0"/>
         <v>38.11308965948141</v>
       </c>
       <c r="N30" s="1">
@@ -2224,10 +2225,10 @@
         <v>30</v>
       </c>
       <c r="G31" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H31" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I31">
         <v>10123</v>
@@ -2242,7 +2243,7 @@
         <v>345</v>
       </c>
       <c r="M31">
-        <f>K31*((1*10^6)/(L31*660))</f>
+        <f t="shared" si="0"/>
         <v>84.321475625823453</v>
       </c>
       <c r="N31" s="1">
@@ -2296,7 +2297,7 @@
         <v>398</v>
       </c>
       <c r="M32">
-        <f>K32*((1*10^6)/(L32*660))</f>
+        <f t="shared" si="0"/>
         <v>61.671996345363176</v>
       </c>
       <c r="N32" s="1">
@@ -2347,7 +2348,7 @@
         <v>372</v>
       </c>
       <c r="M33">
-        <f>K33*((1*10^6)/(L33*660))</f>
+        <f t="shared" si="0"/>
         <v>54.578038449006186</v>
       </c>
       <c r="N33" s="1">
@@ -2380,10 +2381,10 @@
         <v>30</v>
       </c>
       <c r="G34" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H34" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I34">
         <f>9376+1170</f>
@@ -2399,7 +2400,7 @@
         <v>315</v>
       </c>
       <c r="M34">
-        <f>K34*((1*10^6)/(L34*660))</f>
+        <f t="shared" si="0"/>
         <v>19.817219817219819</v>
       </c>
       <c r="N34" s="1">
@@ -2432,10 +2433,10 @@
         <v>30</v>
       </c>
       <c r="G35" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H35" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I35">
         <v>11989</v>
@@ -2450,7 +2451,7 @@
         <v>321</v>
       </c>
       <c r="M35">
-        <f>K35*((1*10^6)/(L35*660))</f>
+        <f t="shared" si="0"/>
         <v>30.20862833946946</v>
       </c>
       <c r="N35" s="1">
@@ -2483,7 +2484,7 @@
         <v>30</v>
       </c>
       <c r="G36" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H36" t="s">
         <v>33</v>
@@ -2502,7 +2503,7 @@
         <v>283</v>
       </c>
       <c r="M36">
-        <f>K36*((1*10^6)/(L36*660))</f>
+        <f t="shared" si="0"/>
         <v>47.328407752436021</v>
       </c>
       <c r="N36" s="1">
@@ -2535,7 +2536,7 @@
         <v>30</v>
       </c>
       <c r="G37" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H37" t="s">
         <v>33</v>
@@ -2553,7 +2554,7 @@
         <v>292</v>
       </c>
       <c r="M37">
-        <f>K37*((1*10^6)/(L37*660))</f>
+        <f t="shared" si="0"/>
         <v>61.228725612287263</v>
       </c>
       <c r="N37" s="1">
@@ -2586,10 +2587,10 @@
         <v>30</v>
       </c>
       <c r="G38" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H38" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I38" s="2">
         <v>10105</v>
@@ -2604,7 +2605,7 @@
         <v>291</v>
       </c>
       <c r="M38">
-        <f>K38*((1*10^6)/(L38*660))</f>
+        <f t="shared" si="0"/>
         <v>79.662605435801325</v>
       </c>
       <c r="N38" s="1">
@@ -2637,10 +2638,10 @@
         <v>30</v>
       </c>
       <c r="G39" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H39" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I39" s="2">
         <v>10250</v>
@@ -2655,7 +2656,7 @@
         <v>308</v>
       </c>
       <c r="M39">
-        <f>K39*((1*10^6)/(L39*660))</f>
+        <f t="shared" si="0"/>
         <v>67.88665879574971</v>
       </c>
       <c r="N39" s="1">
@@ -2688,7 +2689,7 @@
         <v>30</v>
       </c>
       <c r="G40" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H40" t="s">
         <v>33</v>
@@ -2706,7 +2707,7 @@
         <v>286</v>
       </c>
       <c r="M40">
-        <f>K40*((1*10^6)/(L40*660))</f>
+        <f t="shared" si="0"/>
         <v>48.527230345412164</v>
       </c>
       <c r="N40" s="1">
@@ -2739,7 +2740,7 @@
         <v>30</v>
       </c>
       <c r="G41" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H41" t="s">
         <v>33</v>
@@ -2757,7 +2758,7 @@
         <v>290</v>
       </c>
       <c r="M41">
-        <f>K41*((1*10^6)/(L41*660))</f>
+        <f t="shared" si="0"/>
         <v>49.007314524555909</v>
       </c>
       <c r="N41" s="1">
@@ -2771,7 +2772,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:CU1" xr:uid="{7397F12F-A204-1D49-964F-5874A9F571F1}">
+  <autoFilter ref="A1:CU41" xr:uid="{7397F12F-A204-1D49-964F-5874A9F571F1}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:CU41">
       <sortCondition descending="1" ref="C1:C41"/>
     </sortState>

</xml_diff>

<commit_message>
added PCA plots focused on BrdU+ monocytes. SIVE BrdU+ monos cluster pretty distinctly from SIVnoE BrdU+ monos at 21dpi, and then expression profiles get more similar towards necropsy. A high priority for differential expression analysis is SIVE vs SIVnoE at 21dpi.
</commit_message>
<xml_diff>
--- a/data/library_info.xlsx
+++ b/data/library_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewding/Desktop/Projects/2023 BrdU RNAseq/Analyses/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0233EF-1614-974B-BB64-D4E37652A8F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9815EC6-48FA-4145-BA4D-FA1D2F17C14E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1940" yWindow="0" windowWidth="27240" windowHeight="15140" xr2:uid="{80E030B8-BC9B-3D4F-89F4-4C59C10CB779}"/>
   </bookViews>
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="47">
   <si>
     <t>Animal</t>
   </si>
@@ -660,10 +660,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7397F12F-A204-1D49-964F-5874A9F571F1}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:CU41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -825,7 +826,7 @@
         <v>45440</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -876,7 +877,7 @@
         <v>45440</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -927,7 +928,7 @@
         <v>45440</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -978,7 +979,7 @@
         <v>45440</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1029,15 +1030,15 @@
         <v>45440</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
-        <v>7</v>
+      <c r="C8">
+        <v>0</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
@@ -1080,15 +1081,15 @@
         <v>45440</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
-      <c r="C9" t="s">
-        <v>7</v>
+      <c r="C9">
+        <v>0</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
@@ -1131,15 +1132,15 @@
         <v>45440</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
       </c>
-      <c r="C10" t="s">
-        <v>7</v>
+      <c r="C10">
+        <v>0</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
@@ -1182,15 +1183,15 @@
         <v>45462</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>17</v>
       </c>
-      <c r="C11" t="s">
-        <v>7</v>
+      <c r="C11">
+        <v>0</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
@@ -1233,15 +1234,15 @@
         <v>45462</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>15</v>
       </c>
       <c r="B12" t="s">
         <v>34</v>
       </c>
-      <c r="C12" t="s">
-        <v>7</v>
+      <c r="C12">
+        <v>0</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
@@ -1284,15 +1285,15 @@
         <v>45462</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>16</v>
       </c>
       <c r="B13" t="s">
         <v>34</v>
       </c>
-      <c r="C13" t="s">
-        <v>7</v>
+      <c r="C13">
+        <v>0</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
@@ -1335,7 +1336,7 @@
         <v>45462</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>17</v>
       </c>
@@ -1386,7 +1387,7 @@
         <v>45462</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>18</v>
       </c>
@@ -1437,15 +1438,15 @@
         <v>45462</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>23</v>
       </c>
       <c r="B16" t="s">
         <v>35</v>
       </c>
-      <c r="C16" t="s">
-        <v>7</v>
+      <c r="C16">
+        <v>0</v>
       </c>
       <c r="D16" t="s">
         <v>11</v>
@@ -1488,15 +1489,15 @@
         <v>45471</v>
       </c>
     </row>
-    <row r="17" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:99" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>24</v>
       </c>
       <c r="B17" t="s">
         <v>35</v>
       </c>
-      <c r="C17" t="s">
-        <v>7</v>
+      <c r="C17">
+        <v>0</v>
       </c>
       <c r="D17" t="s">
         <v>12</v>
@@ -1539,7 +1540,7 @@
         <v>45471</v>
       </c>
     </row>
-    <row r="18" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:99" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>25</v>
       </c>
@@ -1591,7 +1592,7 @@
         <v>45471</v>
       </c>
     </row>
-    <row r="19" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:99" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>26</v>
       </c>
@@ -1642,7 +1643,7 @@
         <v>45471</v>
       </c>
     </row>
-    <row r="20" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:99" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>27</v>
       </c>
@@ -1694,7 +1695,7 @@
         <v>45471</v>
       </c>
     </row>
-    <row r="21" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:99" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>28</v>
       </c>
@@ -1745,7 +1746,7 @@
         <v>45471</v>
       </c>
     </row>
-    <row r="22" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:99" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>29</v>
       </c>
@@ -1797,7 +1798,7 @@
         <v>45471</v>
       </c>
     </row>
-    <row r="23" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:99" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>30</v>
       </c>
@@ -1848,15 +1849,15 @@
         <v>45471</v>
       </c>
     </row>
-    <row r="24" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:99" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>31</v>
       </c>
       <c r="B24" t="s">
         <v>36</v>
       </c>
-      <c r="C24" t="s">
-        <v>7</v>
+      <c r="C24">
+        <v>0</v>
       </c>
       <c r="D24" t="s">
         <v>11</v>
@@ -1899,15 +1900,15 @@
         <v>45473</v>
       </c>
     </row>
-    <row r="25" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:99" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>32</v>
       </c>
       <c r="B25" t="s">
         <v>36</v>
       </c>
-      <c r="C25" t="s">
-        <v>7</v>
+      <c r="C25">
+        <v>0</v>
       </c>
       <c r="D25" t="s">
         <v>12</v>
@@ -1950,7 +1951,7 @@
         <v>45473</v>
       </c>
     </row>
-    <row r="26" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:99" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>33</v>
       </c>
@@ -2001,7 +2002,7 @@
         <v>45473</v>
       </c>
     </row>
-    <row r="27" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:99" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>34</v>
       </c>
@@ -2052,15 +2053,15 @@
         <v>45473</v>
       </c>
     </row>
-    <row r="28" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:99" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>37</v>
       </c>
       <c r="B28" t="s">
         <v>37</v>
       </c>
-      <c r="C28" t="s">
-        <v>7</v>
+      <c r="C28">
+        <v>0</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
@@ -2103,15 +2104,15 @@
         <v>45473</v>
       </c>
     </row>
-    <row r="29" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:99" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>38</v>
       </c>
       <c r="B29" t="s">
         <v>37</v>
       </c>
-      <c r="C29" t="s">
-        <v>7</v>
+      <c r="C29">
+        <v>0</v>
       </c>
       <c r="D29" t="s">
         <v>12</v>
@@ -2259,7 +2260,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:99" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>13</v>
       </c>
@@ -2310,7 +2311,7 @@
         <v>45462</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>14</v>
       </c>
@@ -2361,7 +2362,7 @@
         <v>45462</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>35</v>
       </c>
@@ -2413,7 +2414,7 @@
         <v>45473</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>36</v>
       </c>
@@ -2464,7 +2465,7 @@
         <v>45473</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>39</v>
       </c>
@@ -2516,7 +2517,7 @@
         <v>45473</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>40</v>
       </c>
@@ -2567,7 +2568,7 @@
         <v>45473</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>41</v>
       </c>
@@ -2618,7 +2619,7 @@
         <v>45473</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>42</v>
       </c>
@@ -2669,7 +2670,7 @@
         <v>45473</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>43</v>
       </c>
@@ -2720,7 +2721,7 @@
         <v>45473</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>44</v>
       </c>
@@ -2773,6 +2774,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:CU41" xr:uid="{7397F12F-A204-1D49-964F-5874A9F571F1}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="MK35"/>
+      </filters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:CU41">
       <sortCondition descending="1" ref="C1:C41"/>
     </sortState>

</xml_diff>